<commit_message>
overview table for appendix
</commit_message>
<xml_diff>
--- a/data/EMMA_ES_data.xlsx
+++ b/data/EMMA_ES_data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/au161118/Dropbox/ASB/Admin stuff/Posters &amp; Papers/PAPERS/EMMA/scripts/emma/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55FAA5B-F241-BF4E-BE8F-D7917D6B3DAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83923D9-981F-E944-A52A-3041ABE3EFFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EMMA_ES_data" sheetId="1" r:id="rId1"/>
+    <sheet name="EMMA_ES_data" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -381,193 +381,193 @@
     <t>Ares et al. 2014</t>
   </si>
   <si>
-    <t>bibtex</t>
-  </si>
-  <si>
-    <t>ashby2015</t>
-  </si>
-  <si>
-    <t>atalay2012a</t>
-  </si>
-  <si>
-    <t>bagger2016</t>
-  </si>
-  <si>
-    <t>behe2014</t>
-  </si>
-  <si>
-    <t>behe2015</t>
-  </si>
-  <si>
-    <t>behe2017</t>
-  </si>
-  <si>
-    <t>bialkova2014a</t>
-  </si>
-  <si>
-    <t>bialkova2011</t>
-  </si>
-  <si>
-    <t>brandstatter2014</t>
-  </si>
-  <si>
-    <t>cavanagh2014</t>
-  </si>
-  <si>
-    <t>chandon2009a</t>
-  </si>
-  <si>
-    <t>du2014</t>
-  </si>
-  <si>
-    <t>fiedler2012</t>
-  </si>
-  <si>
-    <t>folke2016</t>
-  </si>
-  <si>
-    <t>gidlof2013</t>
-  </si>
-  <si>
-    <t>gidlof2017a</t>
-  </si>
-  <si>
-    <t>glaholt2009a</t>
-  </si>
-  <si>
-    <t>glaholt2009b</t>
-  </si>
-  <si>
-    <t>glaholt2012</t>
-  </si>
-  <si>
-    <t>glaholt2010</t>
-  </si>
-  <si>
-    <t>glaholt2009c</t>
-  </si>
-  <si>
-    <t>graham2016</t>
-  </si>
-  <si>
-    <t>grebitus2015</t>
-  </si>
-  <si>
-    <t>guyader2017</t>
-  </si>
-  <si>
     <t>Guyader et al. 2017</t>
   </si>
   <si>
-    <t>hong2016a</t>
-  </si>
-  <si>
-    <t>huang2011</t>
-  </si>
-  <si>
-    <t>hwang2017</t>
-  </si>
-  <si>
-    <t>keller2014</t>
-  </si>
-  <si>
-    <t>kim2012a</t>
-  </si>
-  <si>
-    <t>krajbich2010a</t>
-  </si>
-  <si>
-    <t>kreplin2014a</t>
-  </si>
-  <si>
-    <t>leboeuf2016</t>
-  </si>
-  <si>
     <t>Leboeuf et al. 2016</t>
   </si>
   <si>
-    <t>lohse1997a</t>
-  </si>
-  <si>
-    <t>lindner2014</t>
-  </si>
-  <si>
-    <t>meissner2016b</t>
-  </si>
-  <si>
-    <t>meissner2016a</t>
-  </si>
-  <si>
-    <t>miller2015</t>
-  </si>
-  <si>
-    <t>mitsuda2014</t>
-  </si>
-  <si>
-    <t>nittono2009</t>
-  </si>
-  <si>
-    <t>orquin2015a</t>
-  </si>
-  <si>
-    <t>orquin2019a</t>
-  </si>
-  <si>
-    <t>orquin2020osfb</t>
-  </si>
-  <si>
-    <t>orquin2013</t>
-  </si>
-  <si>
-    <t>paernamets2015a</t>
-  </si>
-  <si>
     <t>Paernamets et al. 2015 Study 1</t>
   </si>
   <si>
     <t>Paernamets et al. 2015 Study 2</t>
   </si>
   <si>
-    <t>pieters1999</t>
-  </si>
-  <si>
-    <t>rubaltelli2012</t>
-  </si>
-  <si>
-    <t>schotter2010a</t>
-  </si>
-  <si>
-    <t>schotter2012a</t>
-  </si>
-  <si>
-    <t>spinks2016a</t>
-  </si>
-  <si>
-    <t>su2013</t>
-  </si>
-  <si>
-    <t>turner2014</t>
-  </si>
-  <si>
-    <t>vanloo2015</t>
-  </si>
-  <si>
-    <t>vanderlaan2015</t>
-  </si>
-  <si>
-    <t>vanderlaan2017</t>
-  </si>
-  <si>
-    <t>wastlund2015</t>
-  </si>
-  <si>
-    <t>wolfson2017</t>
-  </si>
-  <si>
-    <t>vanherpen2011</t>
+    <t>Authors</t>
   </si>
   <si>
     <t>\cite{ares2014}</t>
+  </si>
+  <si>
+    <t>\cite{ashby2015}</t>
+  </si>
+  <si>
+    <t>\cite{atalay2012a}</t>
+  </si>
+  <si>
+    <t>\cite{bagger2016}</t>
+  </si>
+  <si>
+    <t>\cite{behe2014}</t>
+  </si>
+  <si>
+    <t>\cite{behe2015}</t>
+  </si>
+  <si>
+    <t>\cite{behe2017}</t>
+  </si>
+  <si>
+    <t>\cite{bialkova2011}</t>
+  </si>
+  <si>
+    <t>\cite{bialkova2014a}</t>
+  </si>
+  <si>
+    <t>\cite{brandstatter2014}</t>
+  </si>
+  <si>
+    <t>\cite{cavanagh2014}</t>
+  </si>
+  <si>
+    <t>\cite{chandon2009a}</t>
+  </si>
+  <si>
+    <t>\cite{du2014}</t>
+  </si>
+  <si>
+    <t>\cite{fiedler2012}</t>
+  </si>
+  <si>
+    <t>\cite{folke2016}</t>
+  </si>
+  <si>
+    <t>\cite{gidlof2013}</t>
+  </si>
+  <si>
+    <t>\cite{gidlof2017a}</t>
+  </si>
+  <si>
+    <t>\cite{glaholt2009a}</t>
+  </si>
+  <si>
+    <t>\cite{glaholt2009b}</t>
+  </si>
+  <si>
+    <t>\cite{glaholt2012}</t>
+  </si>
+  <si>
+    <t>\cite{glaholt2009c}</t>
+  </si>
+  <si>
+    <t>\cite{glaholt2010}</t>
+  </si>
+  <si>
+    <t>\cite{graham2016}</t>
+  </si>
+  <si>
+    <t>\cite{grebitus2015}</t>
+  </si>
+  <si>
+    <t>\cite{guyader2017}</t>
+  </si>
+  <si>
+    <t>\cite{hong2016a}</t>
+  </si>
+  <si>
+    <t>\cite{huang2011}</t>
+  </si>
+  <si>
+    <t>\cite{hwang2017}</t>
+  </si>
+  <si>
+    <t>\cite{keller2014}</t>
+  </si>
+  <si>
+    <t>\cite{kim2012a}</t>
+  </si>
+  <si>
+    <t>\cite{krajbich2010a}</t>
+  </si>
+  <si>
+    <t>\cite{kreplin2014a}</t>
+  </si>
+  <si>
+    <t>\cite{leboeuf2016}</t>
+  </si>
+  <si>
+    <t>\cite{lindner2014}</t>
+  </si>
+  <si>
+    <t>\cite{lohse1997a}</t>
+  </si>
+  <si>
+    <t>\cite{meissner2016b}</t>
+  </si>
+  <si>
+    <t>\cite{meissner2016a}</t>
+  </si>
+  <si>
+    <t>\cite{miller2015}</t>
+  </si>
+  <si>
+    <t>\cite{mitsuda2014}</t>
+  </si>
+  <si>
+    <t>\cite{nittono2009}</t>
+  </si>
+  <si>
+    <t>\cite{orquin2015a}</t>
+  </si>
+  <si>
+    <t>\cite{orquin2019a}</t>
+  </si>
+  <si>
+    <t>\cite{orquin2020osfb}</t>
+  </si>
+  <si>
+    <t>\cite{orquin2013}</t>
+  </si>
+  <si>
+    <t>\cite{paernamets2015a}</t>
+  </si>
+  <si>
+    <t>\cite{pieters1999}</t>
+  </si>
+  <si>
+    <t>\cite{rubaltelli2012}</t>
+  </si>
+  <si>
+    <t>\cite{schotter2010a}</t>
+  </si>
+  <si>
+    <t>\cite{schotter2012a}</t>
+  </si>
+  <si>
+    <t>\cite{spinks2016a}</t>
+  </si>
+  <si>
+    <t>\cite{su2013}</t>
+  </si>
+  <si>
+    <t>\cite{turner2014}</t>
+  </si>
+  <si>
+    <t>\cite{vanloo2015}</t>
+  </si>
+  <si>
+    <t>\cite{vanderlaan2015}</t>
+  </si>
+  <si>
+    <t>\cite{vanderlaan2017}</t>
+  </si>
+  <si>
+    <t>\cite{wastlund2015}</t>
+  </si>
+  <si>
+    <t>\cite{wolfson2017}</t>
+  </si>
+  <si>
+    <t>\cite{vanherpen2011}</t>
   </si>
 </sst>
 </file>
@@ -1407,18 +1407,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB074C6-C558-E84F-8958-923D6AE15933}">
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="216" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
         <v>116</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -1511,7 +1511,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -1615,7 +1615,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -1647,7 +1647,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
@@ -1743,7 +1743,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
@@ -1792,7 +1792,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
@@ -1847,7 +1847,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -1876,7 +1876,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
         <v>38</v>
@@ -1905,7 +1905,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
@@ -1928,7 +1928,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
         <v>42</v>
@@ -1951,7 +1951,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B25" t="s">
         <v>50</v>
@@ -2098,7 +2098,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
         <v>52</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
         <v>53</v>
@@ -2167,7 +2167,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s">
         <v>54</v>
@@ -2196,7 +2196,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B30" t="s">
         <v>56</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B31" t="s">
         <v>56</v>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B32" t="s">
         <v>56</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B33" t="s">
         <v>56</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
         <v>56</v>
@@ -2314,7 +2314,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B35" t="s">
         <v>58</v>
@@ -2340,7 +2340,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B36" t="s">
         <v>60</v>
@@ -2366,7 +2366,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B37" t="s">
         <v>60</v>
@@ -2392,7 +2392,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B38" t="s">
         <v>60</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="B39" t="s">
         <v>62</v>
@@ -2450,7 +2450,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B40" t="s">
         <v>63</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B41" t="s">
         <v>63</v>
@@ -2508,7 +2508,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B42" t="s">
         <v>64</v>
@@ -2531,7 +2531,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B43" t="s">
         <v>65</v>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B44" t="s">
         <v>65</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B45" t="s">
         <v>66</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B46" t="s">
         <v>67</v>
@@ -2629,10 +2629,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B47" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="C47" t="s">
         <v>35</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B48" t="s">
         <v>69</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B49" t="s">
         <v>70</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B50" t="s">
         <v>71</v>
@@ -2733,7 +2733,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B51" t="s">
         <v>73</v>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B52" t="s">
         <v>75</v>
@@ -2788,7 +2788,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B53" t="s">
         <v>76</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B54" t="s">
         <v>78</v>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B55" t="s">
         <v>78</v>
@@ -2863,10 +2863,10 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B56" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="C56" t="s">
         <v>35</v>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B57" t="s">
         <v>80</v>
@@ -2912,7 +2912,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B58" t="s">
         <v>80</v>
@@ -2938,7 +2938,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B59" t="s">
         <v>81</v>
@@ -2964,7 +2964,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B60" t="s">
         <v>81</v>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B61" t="s">
         <v>83</v>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B62" t="s">
         <v>84</v>
@@ -3039,7 +3039,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B63" t="s">
         <v>84</v>
@@ -3065,7 +3065,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B64" t="s">
         <v>84</v>
@@ -3091,7 +3091,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B65" t="s">
         <v>85</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B66" t="s">
         <v>85</v>
@@ -3140,7 +3140,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B67" t="s">
         <v>85</v>
@@ -3166,7 +3166,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B68" t="s">
         <v>86</v>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B69" t="s">
         <v>86</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B70" t="s">
         <v>86</v>
@@ -3238,7 +3238,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B71" t="s">
         <v>87</v>
@@ -3264,7 +3264,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B72" t="s">
         <v>88</v>
@@ -3290,7 +3290,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B73" t="s">
         <v>89</v>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B74" t="s">
         <v>89</v>
@@ -3345,7 +3345,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B75" t="s">
         <v>91</v>
@@ -3377,7 +3377,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B76" t="s">
         <v>91</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B77" t="s">
         <v>92</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B78" t="s">
         <v>92</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B79" t="s">
         <v>92</v>
@@ -3505,7 +3505,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B80" t="s">
         <v>92</v>
@@ -3537,7 +3537,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B81" t="s">
         <v>93</v>
@@ -3569,7 +3569,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B82" t="s">
         <v>93</v>
@@ -3601,7 +3601,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B83" t="s">
         <v>93</v>
@@ -3633,7 +3633,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B84" t="s">
         <v>93</v>
@@ -3665,7 +3665,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B85" t="s">
         <v>93</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B86" t="s">
         <v>94</v>
@@ -3732,7 +3732,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B87" t="s">
         <v>95</v>
@@ -3767,7 +3767,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B88" t="s">
         <v>96</v>
@@ -3802,7 +3802,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B89" t="s">
         <v>97</v>
@@ -3837,7 +3837,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B90" t="s">
         <v>98</v>
@@ -3863,10 +3863,10 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B91" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
       <c r="C91" t="s">
         <v>35</v>
@@ -3889,10 +3889,10 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B92" t="s">
-        <v>165</v>
+        <v>120</v>
       </c>
       <c r="C92" t="s">
         <v>35</v>
@@ -3915,7 +3915,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B93" t="s">
         <v>99</v>
@@ -3938,7 +3938,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B94" t="s">
         <v>100</v>
@@ -3964,7 +3964,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B95" t="s">
         <v>101</v>
@@ -3987,7 +3987,7 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B96" t="s">
         <v>101</v>
@@ -4010,7 +4010,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B97" t="s">
         <v>102</v>
@@ -4033,7 +4033,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B98" t="s">
         <v>103</v>
@@ -4059,7 +4059,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B99" t="s">
         <v>104</v>
@@ -4085,7 +4085,7 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B100" t="s">
         <v>105</v>
@@ -4111,7 +4111,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B101" t="s">
         <v>107</v>
@@ -4140,7 +4140,7 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B102" t="s">
         <v>108</v>
@@ -4163,7 +4163,7 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B103" t="s">
         <v>110</v>
@@ -4189,7 +4189,7 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B104" t="s">
         <v>111</v>
@@ -4215,7 +4215,7 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B105" t="s">
         <v>113</v>
@@ -4241,7 +4241,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B106" t="s">
         <v>114</v>
@@ -4267,7 +4267,7 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B107" t="s">
         <v>115</v>
@@ -4295,6 +4295,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixes for longtable issues
</commit_message>
<xml_diff>
--- a/data/EMMA_ES_data.xlsx
+++ b/data/EMMA_ES_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/au161118/Dropbox/ASB/Admin stuff/Posters &amp; Papers/PAPERS/EMMA/scripts/emma/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83923D9-981F-E944-A52A-3041ABE3EFFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A913167-E7F7-8A44-B645-54031F2312B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,9 +444,6 @@
     <t>\cite{gidlof2013}</t>
   </si>
   <si>
-    <t>\cite{gidlof2017a}</t>
-  </si>
-  <si>
     <t>\cite{glaholt2009a}</t>
   </si>
   <si>
@@ -568,6 +565,9 @@
   </si>
   <si>
     <t>\cite{vanherpen2011}</t>
+  </si>
+  <si>
+    <t>\cite{gidloef2017a}</t>
   </si>
 </sst>
 </file>
@@ -1410,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB074C6-C558-E84F-8958-923D6AE15933}">
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="200" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2196,7 +2196,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="B30" t="s">
         <v>56</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="B31" t="s">
         <v>56</v>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="B32" t="s">
         <v>56</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="B33" t="s">
         <v>56</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="B34" t="s">
         <v>56</v>
@@ -2314,7 +2314,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B35" t="s">
         <v>58</v>
@@ -2340,7 +2340,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B36" t="s">
         <v>60</v>
@@ -2366,7 +2366,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
         <v>60</v>
@@ -2392,7 +2392,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B38" t="s">
         <v>60</v>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B39" t="s">
         <v>62</v>
@@ -2450,7 +2450,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B40" t="s">
         <v>63</v>
@@ -2479,7 +2479,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B41" t="s">
         <v>63</v>
@@ -2508,7 +2508,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B42" t="s">
         <v>64</v>
@@ -2531,7 +2531,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B43" t="s">
         <v>65</v>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B44" t="s">
         <v>65</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B45" t="s">
         <v>66</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B46" t="s">
         <v>67</v>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B47" t="s">
         <v>117</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B48" t="s">
         <v>69</v>
@@ -2681,7 +2681,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B49" t="s">
         <v>70</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B50" t="s">
         <v>71</v>
@@ -2733,7 +2733,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B51" t="s">
         <v>73</v>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B52" t="s">
         <v>75</v>
@@ -2788,7 +2788,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B53" t="s">
         <v>76</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B54" t="s">
         <v>78</v>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B55" t="s">
         <v>78</v>
@@ -2863,7 +2863,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B56" t="s">
         <v>118</v>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B57" t="s">
         <v>80</v>
@@ -2912,7 +2912,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B58" t="s">
         <v>80</v>
@@ -2938,7 +2938,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B59" t="s">
         <v>81</v>
@@ -2964,7 +2964,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B60" t="s">
         <v>81</v>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B61" t="s">
         <v>83</v>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B62" t="s">
         <v>84</v>
@@ -3039,7 +3039,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B63" t="s">
         <v>84</v>
@@ -3065,7 +3065,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B64" t="s">
         <v>84</v>
@@ -3091,7 +3091,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B65" t="s">
         <v>85</v>
@@ -3114,7 +3114,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B66" t="s">
         <v>85</v>
@@ -3140,7 +3140,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B67" t="s">
         <v>85</v>
@@ -3166,7 +3166,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B68" t="s">
         <v>86</v>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B69" t="s">
         <v>86</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B70" t="s">
         <v>86</v>
@@ -3238,7 +3238,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B71" t="s">
         <v>87</v>
@@ -3264,7 +3264,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B72" t="s">
         <v>88</v>
@@ -3290,7 +3290,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B73" t="s">
         <v>89</v>
@@ -3316,7 +3316,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B74" t="s">
         <v>89</v>
@@ -3345,7 +3345,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B75" t="s">
         <v>91</v>
@@ -3377,7 +3377,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B76" t="s">
         <v>91</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B77" t="s">
         <v>92</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B78" t="s">
         <v>92</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B79" t="s">
         <v>92</v>
@@ -3505,7 +3505,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B80" t="s">
         <v>92</v>
@@ -3537,7 +3537,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B81" t="s">
         <v>93</v>
@@ -3569,7 +3569,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B82" t="s">
         <v>93</v>
@@ -3601,7 +3601,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B83" t="s">
         <v>93</v>
@@ -3633,7 +3633,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B84" t="s">
         <v>93</v>
@@ -3665,7 +3665,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B85" t="s">
         <v>93</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B86" t="s">
         <v>94</v>
@@ -3732,7 +3732,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B87" t="s">
         <v>95</v>
@@ -3767,7 +3767,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B88" t="s">
         <v>96</v>
@@ -3802,7 +3802,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B89" t="s">
         <v>97</v>
@@ -3837,7 +3837,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B90" t="s">
         <v>98</v>
@@ -3863,7 +3863,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B91" t="s">
         <v>119</v>
@@ -3889,7 +3889,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B92" t="s">
         <v>120</v>
@@ -3915,7 +3915,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B93" t="s">
         <v>99</v>
@@ -3938,7 +3938,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B94" t="s">
         <v>100</v>
@@ -3964,7 +3964,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B95" t="s">
         <v>101</v>
@@ -3987,7 +3987,7 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B96" t="s">
         <v>101</v>
@@ -4010,7 +4010,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B97" t="s">
         <v>102</v>
@@ -4033,7 +4033,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B98" t="s">
         <v>103</v>
@@ -4059,7 +4059,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B99" t="s">
         <v>104</v>
@@ -4085,7 +4085,7 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B100" t="s">
         <v>105</v>
@@ -4111,7 +4111,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B101" t="s">
         <v>107</v>
@@ -4140,7 +4140,7 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B102" t="s">
         <v>108</v>
@@ -4163,7 +4163,7 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B103" t="s">
         <v>110</v>
@@ -4189,7 +4189,7 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B104" t="s">
         <v>111</v>
@@ -4215,7 +4215,7 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B105" t="s">
         <v>113</v>
@@ -4241,7 +4241,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B106" t="s">
         <v>114</v>
@@ -4267,7 +4267,7 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B107" t="s">
         <v>115</v>

</xml_diff>

<commit_message>
updates pub bias + descriptive EM code added
</commit_message>
<xml_diff>
--- a/data/EMMA_ES_data.xlsx
+++ b/data/EMMA_ES_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/au161118/Dropbox/ASB/Admin stuff/Posters &amp; Papers/PAPERS/EMMA/scripts/emma/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A913167-E7F7-8A44-B645-54031F2312B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFD396F-8E7C-5E47-B24C-7A9AA48E4C83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="21620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EMMA_ES_data" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="210">
   <si>
     <t>Study</t>
   </si>
@@ -366,9 +366,6 @@
     <t>Waestlund et al. 2014 Study 2</t>
   </si>
   <si>
-    <t>Tobii Glasses</t>
-  </si>
-  <si>
     <t>Waestlund et al. 2014 Study 3</t>
   </si>
   <si>
@@ -568,6 +565,99 @@
   </si>
   <si>
     <t>\cite{gidloef2017a}</t>
+  </si>
+  <si>
+    <t>Bialkova et al. 2020</t>
+  </si>
+  <si>
+    <t>SMI model unknown (acc &lt; .5)</t>
+  </si>
+  <si>
+    <t>Peschel et al. 2019</t>
+  </si>
+  <si>
+    <t>Jenke et al. 2019</t>
+  </si>
+  <si>
+    <t>Kwak &amp; Huettel 2018</t>
+  </si>
+  <si>
+    <t>risky Gamble</t>
+  </si>
+  <si>
+    <t>Meyerding &amp; Merz 2018</t>
+  </si>
+  <si>
+    <t>Tobii glasses 2</t>
+  </si>
+  <si>
+    <t>Neuhofer et al. 2020</t>
+  </si>
+  <si>
+    <t>Robertson &amp; Lunn 2020</t>
+  </si>
+  <si>
+    <t>EyeLink 1000 Plus (acc &lt; .5)</t>
+  </si>
+  <si>
+    <t>Schoemann et al. 2019</t>
+  </si>
+  <si>
+    <t>EyeLink 1000 (acc = .33)</t>
+  </si>
+  <si>
+    <t>van Loo et al. 2019</t>
+  </si>
+  <si>
+    <t>Zuschke 2020</t>
+  </si>
+  <si>
+    <t>Tobii X60</t>
+  </si>
+  <si>
+    <t>Bogomolova et al. 2020</t>
+  </si>
+  <si>
+    <t>Tobii Glasses 1</t>
+  </si>
+  <si>
+    <t>\cite{bialkova2020}</t>
+  </si>
+  <si>
+    <t>\cite{peschel2019}</t>
+  </si>
+  <si>
+    <t>\cite{jenke2019}</t>
+  </si>
+  <si>
+    <t>\cite{kwak2018}</t>
+  </si>
+  <si>
+    <t>\cite{meyerding2018}</t>
+  </si>
+  <si>
+    <t>\cite{neuhofer2020}</t>
+  </si>
+  <si>
+    <t>\cite{robertson2020}</t>
+  </si>
+  <si>
+    <t>\cite{schoemann2019}</t>
+  </si>
+  <si>
+    <t>\cite{vanloo2019}</t>
+  </si>
+  <si>
+    <t>\cite{zuschke2020}</t>
+  </si>
+  <si>
+    <t>\cite{bogomolova2020}</t>
+  </si>
+  <si>
+    <t>grant</t>
+  </si>
+  <si>
+    <t>public</t>
   </si>
 </sst>
 </file>
@@ -1408,17 +1498,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB074C6-C558-E84F-8958-923D6AE15933}">
-  <dimension ref="A1:K107"/>
+  <dimension ref="A1:M123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="200" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" zoomScale="212" workbookViewId="0">
+      <selection activeCell="M122" sqref="M122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1450,25 +1540,34 @@
       <c r="K1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>208</v>
+      </c>
+      <c r="M1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
       <c r="D2">
-        <v>0.47526711799999999</v>
+        <v>0.32</v>
       </c>
       <c r="E2">
         <v>0.13</v>
       </c>
       <c r="F2">
-        <v>0.47002750599999998</v>
+        <v>0.32</v>
+      </c>
+      <c r="G2">
+        <v>0.32</v>
       </c>
       <c r="H2">
         <v>71</v>
@@ -1482,10 +1581,16 @@
       <c r="K2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -1493,8 +1598,14 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
+      <c r="D3">
+        <v>6.93E-2</v>
+      </c>
+      <c r="E3">
+        <v>5.8999999999999999E-3</v>
+      </c>
       <c r="F3">
-        <v>0.2646</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="H3">
         <v>27</v>
@@ -1508,10 +1619,16 @@
       <c r="K3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -1519,8 +1636,14 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
+      <c r="D4">
+        <v>6.7199999999999996E-2</v>
+      </c>
+      <c r="E4">
+        <v>6.6900000000000001E-2</v>
+      </c>
       <c r="F4">
-        <v>0.441</v>
+        <v>7.2300000000000003E-2</v>
       </c>
       <c r="H4">
         <v>34</v>
@@ -1534,10 +1657,16 @@
       <c r="K4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
@@ -1545,8 +1674,14 @@
       <c r="C5" t="s">
         <v>10</v>
       </c>
+      <c r="D5">
+        <v>0.1036</v>
+      </c>
+      <c r="E5">
+        <v>9.5699999999999993E-2</v>
+      </c>
       <c r="F5">
-        <v>0.68600000000000005</v>
+        <v>0.1062</v>
       </c>
       <c r="H5">
         <v>81</v>
@@ -1560,10 +1695,16 @@
       <c r="K5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -1572,10 +1713,10 @@
         <v>19</v>
       </c>
       <c r="D6">
-        <v>0.19</v>
+        <v>0.18709999999999999</v>
       </c>
       <c r="F6">
-        <v>0.14000000000000001</v>
+        <v>0.1449</v>
       </c>
       <c r="H6">
         <v>63</v>
@@ -1586,10 +1727,16 @@
       <c r="J6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -1598,10 +1745,10 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>0.15</v>
+        <v>0.15490000000000001</v>
       </c>
       <c r="F7">
-        <v>0.14000000000000001</v>
+        <v>0.13780000000000001</v>
       </c>
       <c r="H7">
         <v>64</v>
@@ -1612,10 +1759,16 @@
       <c r="J7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -1644,10 +1797,16 @@
       <c r="K8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -1676,10 +1835,16 @@
       <c r="K9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
@@ -1708,10 +1873,16 @@
       <c r="K10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
@@ -1740,10 +1911,16 @@
       <c r="K11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
@@ -1766,10 +1943,16 @@
       <c r="K12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
@@ -1789,10 +1972,16 @@
       <c r="J13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
@@ -1815,10 +2004,16 @@
       <c r="K14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
@@ -1844,10 +2039,16 @@
       <c r="K15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -1873,10 +2074,16 @@
       <c r="K16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B17" t="s">
         <v>38</v>
@@ -1902,10 +2109,16 @@
       <c r="K17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
@@ -1925,10 +2138,16 @@
       <c r="J18" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B19" t="s">
         <v>42</v>
@@ -1948,10 +2167,16 @@
       <c r="J19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
@@ -1971,10 +2196,16 @@
       <c r="J20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
@@ -1994,10 +2225,16 @@
       <c r="J21" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
@@ -2017,10 +2254,16 @@
       <c r="J22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
@@ -2043,10 +2286,16 @@
       <c r="K23" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B24" t="s">
         <v>48</v>
@@ -2072,10 +2321,16 @@
       <c r="K24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B25" t="s">
         <v>50</v>
@@ -2095,10 +2350,16 @@
       <c r="J25" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
@@ -2118,10 +2379,16 @@
       <c r="J26" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B27" t="s">
         <v>52</v>
@@ -2141,10 +2408,16 @@
       <c r="J27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B28" t="s">
         <v>53</v>
@@ -2164,10 +2437,16 @@
       <c r="J28" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
         <v>54</v>
@@ -2193,10 +2472,16 @@
       <c r="K29" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B30" t="s">
         <v>56</v>
@@ -2204,11 +2489,14 @@
       <c r="C30" t="s">
         <v>32</v>
       </c>
+      <c r="F30">
+        <v>0.2</v>
+      </c>
       <c r="G30">
-        <v>0.99808456599999995</v>
+        <v>0.2</v>
       </c>
       <c r="H30">
-        <v>50</v>
+        <v>260</v>
       </c>
       <c r="I30" t="s">
         <v>57</v>
@@ -2216,10 +2504,16 @@
       <c r="J30" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B31" t="s">
         <v>56</v>
@@ -2231,7 +2525,7 @@
         <v>0.54</v>
       </c>
       <c r="H31">
-        <v>38</v>
+        <v>260</v>
       </c>
       <c r="I31" t="s">
         <v>57</v>
@@ -2239,10 +2533,16 @@
       <c r="J31" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B32" t="s">
         <v>56</v>
@@ -2254,7 +2554,7 @@
         <v>9.9667994999999995E-2</v>
       </c>
       <c r="H32">
-        <v>50</v>
+        <v>260</v>
       </c>
       <c r="I32" t="s">
         <v>57</v>
@@ -2265,10 +2565,16 @@
       <c r="K32" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B33" t="s">
         <v>56</v>
@@ -2280,7 +2586,7 @@
         <v>0.02</v>
       </c>
       <c r="H33">
-        <v>38</v>
+        <v>260</v>
       </c>
       <c r="I33" t="s">
         <v>57</v>
@@ -2288,10 +2594,16 @@
       <c r="J33" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B34" t="s">
         <v>56</v>
@@ -2303,7 +2615,7 @@
         <v>0.48</v>
       </c>
       <c r="H34">
-        <v>38</v>
+        <v>260</v>
       </c>
       <c r="I34" t="s">
         <v>57</v>
@@ -2311,10 +2623,16 @@
       <c r="J34" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B35" t="s">
         <v>58</v>
@@ -2337,10 +2655,16 @@
       <c r="K35" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B36" t="s">
         <v>60</v>
@@ -2363,10 +2687,16 @@
       <c r="J36" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B37" t="s">
         <v>60</v>
@@ -2389,10 +2719,16 @@
       <c r="J37" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B38" t="s">
         <v>60</v>
@@ -2418,10 +2754,16 @@
       <c r="K38" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
         <v>62</v>
@@ -2447,10 +2789,16 @@
       <c r="K39" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B40" t="s">
         <v>63</v>
@@ -2476,10 +2824,16 @@
       <c r="J40" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B41" t="s">
         <v>63</v>
@@ -2505,10 +2859,16 @@
       <c r="K41" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B42" t="s">
         <v>64</v>
@@ -2528,10 +2888,16 @@
       <c r="J42" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B43" t="s">
         <v>65</v>
@@ -2554,10 +2920,16 @@
       <c r="J43" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B44" t="s">
         <v>65</v>
@@ -2577,10 +2949,16 @@
       <c r="J44" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B45" t="s">
         <v>66</v>
@@ -2600,10 +2978,16 @@
       <c r="J45" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B46" t="s">
         <v>67</v>
@@ -2626,13 +3010,19 @@
       <c r="K46" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C47" t="s">
         <v>35</v>
@@ -2652,10 +3042,16 @@
       <c r="K47" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B48" t="s">
         <v>69</v>
@@ -2678,10 +3074,16 @@
       <c r="K48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B49" t="s">
         <v>70</v>
@@ -2704,10 +3106,16 @@
       <c r="K49" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B50" t="s">
         <v>71</v>
@@ -2730,10 +3138,16 @@
       <c r="K50" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B51" t="s">
         <v>73</v>
@@ -2756,10 +3170,16 @@
       <c r="K51" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B52" t="s">
         <v>75</v>
@@ -2785,10 +3205,16 @@
       <c r="K52" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B53" t="s">
         <v>76</v>
@@ -2808,10 +3234,16 @@
       <c r="J53" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B54" t="s">
         <v>78</v>
@@ -2834,10 +3266,16 @@
       <c r="J54" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B55" t="s">
         <v>78</v>
@@ -2860,19 +3298,28 @@
       <c r="J55" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C56" t="s">
         <v>35</v>
       </c>
       <c r="E56">
-        <v>0.74392350600000001</v>
+        <v>0.67</v>
+      </c>
+      <c r="F56">
+        <v>0.26</v>
       </c>
       <c r="H56">
         <v>54</v>
@@ -2886,10 +3333,16 @@
       <c r="K56" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B57" t="s">
         <v>80</v>
@@ -2909,10 +3362,16 @@
       <c r="J57" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B58" t="s">
         <v>80</v>
@@ -2921,7 +3380,7 @@
         <v>10</v>
       </c>
       <c r="F58">
-        <v>0.88543774500000005</v>
+        <v>0.57310000000000005</v>
       </c>
       <c r="H58">
         <v>26</v>
@@ -2935,10 +3394,16 @@
       <c r="K58" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B59" t="s">
         <v>81</v>
@@ -2961,10 +3426,16 @@
       <c r="J59" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B60" t="s">
         <v>81</v>
@@ -2984,10 +3455,16 @@
       <c r="J60" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L60">
+        <v>1</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B61" t="s">
         <v>83</v>
@@ -2996,10 +3473,7 @@
         <v>68</v>
       </c>
       <c r="D61">
-        <v>0.69046264599999996</v>
-      </c>
-      <c r="E61">
-        <v>0.83934049700000002</v>
+        <v>0.42</v>
       </c>
       <c r="H61">
         <v>40</v>
@@ -3013,10 +3487,16 @@
       <c r="K61" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B62" t="s">
         <v>84</v>
@@ -3036,10 +3516,16 @@
       <c r="J62" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B63" t="s">
         <v>84</v>
@@ -3062,10 +3548,16 @@
       <c r="K63" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B64" t="s">
         <v>84</v>
@@ -3088,10 +3580,16 @@
       <c r="K64" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B65" t="s">
         <v>85</v>
@@ -3111,10 +3609,16 @@
       <c r="J65" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B66" t="s">
         <v>85</v>
@@ -3137,10 +3641,16 @@
       <c r="K66" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B67" t="s">
         <v>85</v>
@@ -3163,10 +3673,16 @@
       <c r="K67" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L67">
+        <v>0</v>
+      </c>
+      <c r="M67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B68" t="s">
         <v>86</v>
@@ -3183,10 +3699,16 @@
       <c r="J68" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B69" t="s">
         <v>86</v>
@@ -3209,10 +3731,16 @@
       <c r="K69" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B70" t="s">
         <v>86</v>
@@ -3235,10 +3763,16 @@
       <c r="K70" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B71" t="s">
         <v>87</v>
@@ -3261,10 +3795,16 @@
       <c r="K71" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L71">
+        <v>1</v>
+      </c>
+      <c r="M71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B72" t="s">
         <v>88</v>
@@ -3287,10 +3827,16 @@
       <c r="J72" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B73" t="s">
         <v>89</v>
@@ -3313,10 +3859,16 @@
       <c r="J73" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B74" t="s">
         <v>89</v>
@@ -3342,10 +3894,16 @@
       <c r="K74" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B75" t="s">
         <v>91</v>
@@ -3374,10 +3932,16 @@
       <c r="K75" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L75">
+        <v>1</v>
+      </c>
+      <c r="M75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B76" t="s">
         <v>91</v>
@@ -3406,10 +3970,16 @@
       <c r="K76" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L76">
+        <v>1</v>
+      </c>
+      <c r="M76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B77" t="s">
         <v>92</v>
@@ -3438,10 +4008,16 @@
       <c r="K77" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L77">
+        <v>1</v>
+      </c>
+      <c r="M77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B78" t="s">
         <v>92</v>
@@ -3470,10 +4046,16 @@
       <c r="K78" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L78">
+        <v>1</v>
+      </c>
+      <c r="M78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B79" t="s">
         <v>92</v>
@@ -3502,10 +4084,16 @@
       <c r="K79" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="M79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B80" t="s">
         <v>92</v>
@@ -3534,10 +4122,16 @@
       <c r="K80" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="M80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B81" t="s">
         <v>93</v>
@@ -3566,10 +4160,16 @@
       <c r="K81" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L81">
+        <v>1</v>
+      </c>
+      <c r="M81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B82" t="s">
         <v>93</v>
@@ -3598,10 +4198,16 @@
       <c r="K82" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L82">
+        <v>1</v>
+      </c>
+      <c r="M82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B83" t="s">
         <v>93</v>
@@ -3630,10 +4236,16 @@
       <c r="K83" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L83">
+        <v>1</v>
+      </c>
+      <c r="M83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B84" t="s">
         <v>93</v>
@@ -3662,10 +4274,16 @@
       <c r="K84" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L84">
+        <v>1</v>
+      </c>
+      <c r="M84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B85" t="s">
         <v>93</v>
@@ -3694,10 +4312,16 @@
       <c r="K85" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L85">
+        <v>1</v>
+      </c>
+      <c r="M85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B86" t="s">
         <v>94</v>
@@ -3706,16 +4330,13 @@
         <v>68</v>
       </c>
       <c r="D86">
-        <v>0.21247129200000001</v>
+        <v>0.42301729999999998</v>
       </c>
       <c r="E86">
-        <v>0.16491060799999999</v>
+        <v>0.41704140000000001</v>
       </c>
       <c r="F86">
-        <v>0.22770894899999999</v>
-      </c>
-      <c r="G86">
-        <v>0.216892371</v>
+        <v>0.47683969999999998</v>
       </c>
       <c r="H86">
         <v>71</v>
@@ -3729,10 +4350,16 @@
       <c r="K86" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B87" t="s">
         <v>95</v>
@@ -3764,10 +4391,16 @@
       <c r="K87" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B88" t="s">
         <v>96</v>
@@ -3799,10 +4432,16 @@
       <c r="K88" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B89" t="s">
         <v>97</v>
@@ -3811,16 +4450,13 @@
         <v>68</v>
       </c>
       <c r="D89">
-        <v>0.24515753800000001</v>
+        <v>0.50791059999999999</v>
       </c>
       <c r="E89">
-        <v>0.179774618</v>
+        <v>0.46335900000000002</v>
       </c>
       <c r="F89">
-        <v>0.24852858899999999</v>
-      </c>
-      <c r="G89">
-        <v>0.230007078</v>
+        <v>0.53509899999999999</v>
       </c>
       <c r="H89">
         <v>68</v>
@@ -3834,10 +4470,16 @@
       <c r="K89" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B90" t="s">
         <v>98</v>
@@ -3860,13 +4502,19 @@
       <c r="K90" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L90">
+        <v>1</v>
+      </c>
+      <c r="M90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B91" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C91" t="s">
         <v>35</v>
@@ -3886,13 +4534,19 @@
       <c r="K91" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L91">
+        <v>1</v>
+      </c>
+      <c r="M91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B92" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C92" t="s">
         <v>35</v>
@@ -3912,10 +4566,16 @@
       <c r="K92" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L92">
+        <v>1</v>
+      </c>
+      <c r="M92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B93" t="s">
         <v>99</v>
@@ -3935,10 +4595,16 @@
       <c r="K93" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B94" t="s">
         <v>100</v>
@@ -3961,10 +4627,16 @@
       <c r="K94" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L94">
+        <v>0</v>
+      </c>
+      <c r="M94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B95" t="s">
         <v>101</v>
@@ -3984,10 +4656,16 @@
       <c r="J95" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L95">
+        <v>1</v>
+      </c>
+      <c r="M95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B96" t="s">
         <v>101</v>
@@ -4007,10 +4685,16 @@
       <c r="J96" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L96">
+        <v>1</v>
+      </c>
+      <c r="M96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B97" t="s">
         <v>102</v>
@@ -4030,10 +4714,16 @@
       <c r="J97" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L97">
+        <v>1</v>
+      </c>
+      <c r="M97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B98" t="s">
         <v>103</v>
@@ -4056,10 +4746,16 @@
       <c r="K98" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B99" t="s">
         <v>104</v>
@@ -4068,7 +4764,7 @@
         <v>35</v>
       </c>
       <c r="E99">
-        <v>0.70710678100000002</v>
+        <v>0.47</v>
       </c>
       <c r="H99">
         <v>49</v>
@@ -4082,10 +4778,16 @@
       <c r="K99" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L99">
+        <v>1</v>
+      </c>
+      <c r="M99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B100" t="s">
         <v>105</v>
@@ -4108,10 +4810,16 @@
       <c r="K100" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B101" t="s">
         <v>107</v>
@@ -4137,10 +4845,16 @@
       <c r="K101" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L101">
+        <v>0</v>
+      </c>
+      <c r="M101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B102" t="s">
         <v>108</v>
@@ -4160,10 +4874,16 @@
       <c r="J102" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L102">
+        <v>1</v>
+      </c>
+      <c r="M102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B103" t="s">
         <v>110</v>
@@ -4186,10 +4906,16 @@
       <c r="K103" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L103">
+        <v>1</v>
+      </c>
+      <c r="M103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B104" t="s">
         <v>111</v>
@@ -4204,7 +4930,7 @@
         <v>98</v>
       </c>
       <c r="I104" t="s">
-        <v>112</v>
+        <v>196</v>
       </c>
       <c r="J104" t="s">
         <v>25</v>
@@ -4212,13 +4938,19 @@
       <c r="K104" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L104">
+        <v>0</v>
+      </c>
+      <c r="M104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B105" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C105" t="s">
         <v>35</v>
@@ -4230,7 +4962,7 @@
         <v>66</v>
       </c>
       <c r="I105" t="s">
-        <v>112</v>
+        <v>196</v>
       </c>
       <c r="J105" t="s">
         <v>25</v>
@@ -4238,13 +4970,19 @@
       <c r="K105" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L105">
+        <v>0</v>
+      </c>
+      <c r="M105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B106" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C106" t="s">
         <v>10</v>
@@ -4264,13 +5002,19 @@
       <c r="K106" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L106">
+        <v>1</v>
+      </c>
+      <c r="M106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B107" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C107" t="s">
         <v>35</v>
@@ -4292,6 +5036,545 @@
       </c>
       <c r="K107" t="s">
         <v>13</v>
+      </c>
+      <c r="L107">
+        <v>1</v>
+      </c>
+      <c r="M107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>197</v>
+      </c>
+      <c r="B108" t="s">
+        <v>179</v>
+      </c>
+      <c r="C108" t="s">
+        <v>35</v>
+      </c>
+      <c r="D108">
+        <v>0.23222319999999999</v>
+      </c>
+      <c r="F108">
+        <v>0.27519729999999998</v>
+      </c>
+      <c r="H108">
+        <v>30</v>
+      </c>
+      <c r="I108" t="s">
+        <v>180</v>
+      </c>
+      <c r="J108" t="s">
+        <v>12</v>
+      </c>
+      <c r="K108" t="s">
+        <v>13</v>
+      </c>
+      <c r="L108">
+        <v>1</v>
+      </c>
+      <c r="M108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>198</v>
+      </c>
+      <c r="B109" t="s">
+        <v>181</v>
+      </c>
+      <c r="C109" t="s">
+        <v>23</v>
+      </c>
+      <c r="D109">
+        <v>3.8813599999999999E-3</v>
+      </c>
+      <c r="E109">
+        <v>1.5072540000000001E-2</v>
+      </c>
+      <c r="F109">
+        <v>1.3343010000000001E-2</v>
+      </c>
+      <c r="H109">
+        <v>127</v>
+      </c>
+      <c r="I109" t="s">
+        <v>11</v>
+      </c>
+      <c r="J109" t="s">
+        <v>12</v>
+      </c>
+      <c r="K109" t="s">
+        <v>13</v>
+      </c>
+      <c r="L109">
+        <v>1</v>
+      </c>
+      <c r="M109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>198</v>
+      </c>
+      <c r="B110" t="s">
+        <v>181</v>
+      </c>
+      <c r="C110" t="s">
+        <v>46</v>
+      </c>
+      <c r="D110">
+        <v>9.7537780000000004E-2</v>
+      </c>
+      <c r="E110">
+        <v>4.5266790000000001E-2</v>
+      </c>
+      <c r="F110">
+        <v>9.6266900000000002E-2</v>
+      </c>
+      <c r="H110">
+        <v>127</v>
+      </c>
+      <c r="I110" t="s">
+        <v>11</v>
+      </c>
+      <c r="J110" t="s">
+        <v>12</v>
+      </c>
+      <c r="K110" t="s">
+        <v>13</v>
+      </c>
+      <c r="L110">
+        <v>1</v>
+      </c>
+      <c r="M110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>199</v>
+      </c>
+      <c r="B111" t="s">
+        <v>182</v>
+      </c>
+      <c r="C111" t="s">
+        <v>10</v>
+      </c>
+      <c r="E111">
+        <v>0.32</v>
+      </c>
+      <c r="H111">
+        <v>122</v>
+      </c>
+      <c r="I111" t="s">
+        <v>11</v>
+      </c>
+      <c r="J111" t="s">
+        <v>59</v>
+      </c>
+      <c r="K111" t="s">
+        <v>13</v>
+      </c>
+      <c r="L111">
+        <v>0</v>
+      </c>
+      <c r="M111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>199</v>
+      </c>
+      <c r="B112" t="s">
+        <v>182</v>
+      </c>
+      <c r="C112" t="s">
+        <v>68</v>
+      </c>
+      <c r="D112">
+        <v>0.23</v>
+      </c>
+      <c r="E112">
+        <v>0.35</v>
+      </c>
+      <c r="H112">
+        <v>122</v>
+      </c>
+      <c r="I112" t="s">
+        <v>11</v>
+      </c>
+      <c r="J112" t="s">
+        <v>59</v>
+      </c>
+      <c r="K112" t="s">
+        <v>13</v>
+      </c>
+      <c r="L112">
+        <v>0</v>
+      </c>
+      <c r="M112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>200</v>
+      </c>
+      <c r="B113" t="s">
+        <v>183</v>
+      </c>
+      <c r="C113" t="s">
+        <v>44</v>
+      </c>
+      <c r="F113">
+        <v>0.44</v>
+      </c>
+      <c r="H113">
+        <v>63</v>
+      </c>
+      <c r="I113" t="s">
+        <v>11</v>
+      </c>
+      <c r="J113" t="s">
+        <v>184</v>
+      </c>
+      <c r="K113" t="s">
+        <v>47</v>
+      </c>
+      <c r="L113">
+        <v>0</v>
+      </c>
+      <c r="M113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>201</v>
+      </c>
+      <c r="B114" t="s">
+        <v>185</v>
+      </c>
+      <c r="C114" t="s">
+        <v>10</v>
+      </c>
+      <c r="F114">
+        <v>0.29139999999999999</v>
+      </c>
+      <c r="H114">
+        <v>73</v>
+      </c>
+      <c r="I114" t="s">
+        <v>186</v>
+      </c>
+      <c r="J114" t="s">
+        <v>12</v>
+      </c>
+      <c r="K114" t="s">
+        <v>13</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+      <c r="M114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>202</v>
+      </c>
+      <c r="B115" t="s">
+        <v>187</v>
+      </c>
+      <c r="C115" t="s">
+        <v>46</v>
+      </c>
+      <c r="F115">
+        <v>0.23</v>
+      </c>
+      <c r="H115">
+        <v>164</v>
+      </c>
+      <c r="I115" t="s">
+        <v>72</v>
+      </c>
+      <c r="J115" t="s">
+        <v>12</v>
+      </c>
+      <c r="K115" t="s">
+        <v>13</v>
+      </c>
+      <c r="L115">
+        <v>1</v>
+      </c>
+      <c r="M115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>203</v>
+      </c>
+      <c r="B116" t="s">
+        <v>188</v>
+      </c>
+      <c r="C116" t="s">
+        <v>44</v>
+      </c>
+      <c r="D116">
+        <v>0.13</v>
+      </c>
+      <c r="G116">
+        <v>0.15</v>
+      </c>
+      <c r="H116">
+        <v>74</v>
+      </c>
+      <c r="I116" t="s">
+        <v>189</v>
+      </c>
+      <c r="J116" t="s">
+        <v>12</v>
+      </c>
+      <c r="K116" t="s">
+        <v>13</v>
+      </c>
+      <c r="L116">
+        <v>1</v>
+      </c>
+      <c r="M116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>204</v>
+      </c>
+      <c r="B117" t="s">
+        <v>190</v>
+      </c>
+      <c r="C117" t="s">
+        <v>35</v>
+      </c>
+      <c r="G117">
+        <v>0.87</v>
+      </c>
+      <c r="H117">
+        <v>40</v>
+      </c>
+      <c r="I117" t="s">
+        <v>191</v>
+      </c>
+      <c r="J117" t="s">
+        <v>184</v>
+      </c>
+      <c r="K117" t="s">
+        <v>13</v>
+      </c>
+      <c r="L117">
+        <v>1</v>
+      </c>
+      <c r="M117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>205</v>
+      </c>
+      <c r="B118" t="s">
+        <v>192</v>
+      </c>
+      <c r="C118" t="s">
+        <v>68</v>
+      </c>
+      <c r="F118">
+        <v>0.1058963</v>
+      </c>
+      <c r="H118">
+        <v>103</v>
+      </c>
+      <c r="I118" t="s">
+        <v>72</v>
+      </c>
+      <c r="J118" t="s">
+        <v>12</v>
+      </c>
+      <c r="K118" t="s">
+        <v>13</v>
+      </c>
+      <c r="L118">
+        <v>0</v>
+      </c>
+      <c r="M118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>205</v>
+      </c>
+      <c r="B119" t="s">
+        <v>192</v>
+      </c>
+      <c r="C119" t="s">
+        <v>10</v>
+      </c>
+      <c r="F119">
+        <v>0.12766169999999999</v>
+      </c>
+      <c r="H119">
+        <v>103</v>
+      </c>
+      <c r="I119" t="s">
+        <v>72</v>
+      </c>
+      <c r="J119" t="s">
+        <v>12</v>
+      </c>
+      <c r="K119" t="s">
+        <v>13</v>
+      </c>
+      <c r="L119">
+        <v>0</v>
+      </c>
+      <c r="M119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>206</v>
+      </c>
+      <c r="B120" t="s">
+        <v>193</v>
+      </c>
+      <c r="C120" t="s">
+        <v>23</v>
+      </c>
+      <c r="E120">
+        <v>0.27208979999999999</v>
+      </c>
+      <c r="H120">
+        <v>172</v>
+      </c>
+      <c r="I120" t="s">
+        <v>194</v>
+      </c>
+      <c r="J120" t="s">
+        <v>12</v>
+      </c>
+      <c r="K120" t="s">
+        <v>13</v>
+      </c>
+      <c r="L120">
+        <v>0</v>
+      </c>
+      <c r="M120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>206</v>
+      </c>
+      <c r="B121" t="s">
+        <v>193</v>
+      </c>
+      <c r="C121" t="s">
+        <v>46</v>
+      </c>
+      <c r="E121">
+        <v>0.31456800000000001</v>
+      </c>
+      <c r="H121">
+        <v>172</v>
+      </c>
+      <c r="I121" t="s">
+        <v>194</v>
+      </c>
+      <c r="J121" t="s">
+        <v>12</v>
+      </c>
+      <c r="K121" t="s">
+        <v>13</v>
+      </c>
+      <c r="L121">
+        <v>0</v>
+      </c>
+      <c r="M121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>206</v>
+      </c>
+      <c r="B122" t="s">
+        <v>193</v>
+      </c>
+      <c r="C122" t="s">
+        <v>68</v>
+      </c>
+      <c r="E122">
+        <v>8.3371139999999996E-2</v>
+      </c>
+      <c r="H122">
+        <v>172</v>
+      </c>
+      <c r="I122" t="s">
+        <v>194</v>
+      </c>
+      <c r="J122" t="s">
+        <v>12</v>
+      </c>
+      <c r="K122" t="s">
+        <v>13</v>
+      </c>
+      <c r="L122">
+        <v>0</v>
+      </c>
+      <c r="M122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>207</v>
+      </c>
+      <c r="B123" t="s">
+        <v>195</v>
+      </c>
+      <c r="C123" t="s">
+        <v>23</v>
+      </c>
+      <c r="D123">
+        <v>0.1377389</v>
+      </c>
+      <c r="H123">
+        <v>200</v>
+      </c>
+      <c r="I123" t="s">
+        <v>49</v>
+      </c>
+      <c r="J123" t="s">
+        <v>12</v>
+      </c>
+      <c r="K123" t="s">
+        <v>13</v>
+      </c>
+      <c r="L123">
+        <v>1</v>
+      </c>
+      <c r="M123">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>